<commit_message>
Update 2020-03-20 #1 - Add rating/device route search implements (for check is deviceId is set) - Add rating/device route save implements (for register/unregister)
</commit_message>
<xml_diff>
--- a/db/Test Scripts/2020-03-19/db_objects.xlsx
+++ b/db/Test Scripts/2020-03-19/db_objects.xlsx
@@ -652,9 +652,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -951,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B196"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="A183" sqref="A183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1027,10 +1028,10 @@
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1051,10 +1052,10 @@
       </c>
     </row>
     <row r="12" spans="1:2">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>